<commit_message>
Modified files to prepare for v0.9.9 release
Modified the ref numbers in the spreadsheet files and the index-dak.md file.
</commit_message>
<xml_diff>
--- a/input/indicators/IMMZ DAK_indicators.xlsx
+++ b/input/indicators/IMMZ DAK_indicators.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldhealthorg.sharepoint.com/sites/DigitalAcceleratorKits/Shared Documents/Immunizations Digital Accelerator Kit/_FINAL spreadsheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WHO\GitHub\smart-dak-immunizations\input\indicators\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{E11CB9A2-C5E4-434F-89F9-1FBF5DB1F617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8DB67663-355F-4866-BAD1-63AAA9CD5321}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3BA4B3A-BC6F-4F1C-BB72-9D5831B7E854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="17" r:id="rId1"/>
@@ -160,10 +160,6 @@
     <t>If there are any other notes or information, it should be noted here. This should include any additional information that does not fit into the other columns</t>
   </si>
   <si>
-    <t>https://smart.who.int/dak-immz/v1.0.0/IMMZ DAK_indicators.xlsx
-© World Health Organization 2024. Some rights reserved. This work is available under the</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 CC BY-NC-SA 3.0 IGO licence</t>
   </si>
@@ -3279,6 +3275,10 @@
       </rPr>
       <t>All references were accessed on 10 July 2024.</t>
     </r>
+  </si>
+  <si>
+    <t>https://smart.who.int/dak-immz/v0.9.9/IMMZ DAK_indicators.xlsx
+© World Health Organization 2024. Some rights reserved. This work is available under the</t>
   </si>
 </sst>
 </file>
@@ -3288,7 +3288,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="41">
+  <fonts count="41" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -3934,24 +3934,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="1" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="40" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3964,8 +3946,26 @@
     <xf numFmtId="0" fontId="39" fillId="9" borderId="6" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="1" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="18" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3988,6 +3988,12 @@
     <xf numFmtId="0" fontId="21" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3999,12 +4005,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -8207,9 +8207,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -8247,7 +8247,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -8353,7 +8353,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -8495,7 +8495,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -8531,78 +8531,76 @@
   </sheetPr>
   <dimension ref="B1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" customWidth="1"/>
-    <col min="2" max="2" width="34.5703125" customWidth="1"/>
-    <col min="3" max="3" width="31.140625" customWidth="1"/>
+    <col min="1" max="1" width="4.26953125" customWidth="1"/>
+    <col min="2" max="2" width="34.54296875" customWidth="1"/>
+    <col min="3" max="3" width="31.1796875" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
     <col min="5" max="5" width="3" customWidth="1"/>
-    <col min="6" max="6" width="3.42578125" customWidth="1"/>
-    <col min="7" max="7" width="42.28515625" customWidth="1"/>
+    <col min="6" max="6" width="3.453125" customWidth="1"/>
+    <col min="7" max="7" width="42.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" s="13" customFormat="1" ht="14.45">
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
+    <row r="1" spans="2:7" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
     </row>
-    <row r="2" spans="2:7" s="13" customFormat="1" ht="14.45">
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
+    <row r="2" spans="2:7" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
     </row>
-    <row r="3" spans="2:7" s="13" customFormat="1" ht="14.45">
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
+    <row r="3" spans="2:7" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
     </row>
-    <row r="4" spans="2:7" s="13" customFormat="1" ht="14.45">
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
+    <row r="4" spans="2:7" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
     </row>
-    <row r="5" spans="2:7" s="13" customFormat="1" ht="14.45">
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
+    <row r="5" spans="2:7" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="B5" s="50"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
     </row>
-    <row r="6" spans="2:7" s="13" customFormat="1" ht="14.45">
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
+    <row r="6" spans="2:7" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
     </row>
-    <row r="7" spans="2:7" s="13" customFormat="1" ht="14.45">
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
+    <row r="7" spans="2:7" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
     </row>
-    <row r="8" spans="2:7" s="13" customFormat="1" ht="14.45">
+    <row r="8" spans="2:7" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
       <c r="D8" s="15"/>
@@ -8610,17 +8608,17 @@
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
     </row>
-    <row r="9" spans="2:7" s="14" customFormat="1" ht="83.25" customHeight="1">
-      <c r="B9" s="46" t="s">
+    <row r="9" spans="2:7" s="14" customFormat="1" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="51"/>
     </row>
-    <row r="10" spans="2:7" s="13" customFormat="1" ht="14.45">
+    <row r="10" spans="2:7" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="B10"/>
       <c r="C10"/>
       <c r="D10"/>
@@ -8628,159 +8626,152 @@
       <c r="F10"/>
       <c r="G10"/>
     </row>
-    <row r="11" spans="2:7" s="13" customFormat="1" ht="14.45">
+    <row r="11" spans="2:7" s="13" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="B11" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="47" t="s">
+      <c r="C11" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="47"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
     </row>
-    <row r="12" spans="2:7" ht="33" customHeight="1">
+    <row r="12" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="42" t="s">
+      <c r="C12" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="44"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="48"/>
     </row>
-    <row r="13" spans="2:7" ht="19.5" customHeight="1">
+    <row r="13" spans="2:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="42" t="s">
+      <c r="C13" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="44"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="48"/>
     </row>
-    <row r="14" spans="2:7" ht="18.75" customHeight="1">
+    <row r="14" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="42" t="s">
+      <c r="C14" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="44"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="48"/>
     </row>
-    <row r="15" spans="2:7" ht="17.25" customHeight="1">
+    <row r="15" spans="2:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="42" t="s">
+      <c r="C15" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="44"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="48"/>
     </row>
-    <row r="16" spans="2:7" ht="51" customHeight="1">
+    <row r="16" spans="2:7" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="42" t="s">
+      <c r="C16" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="44"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="48"/>
     </row>
-    <row r="17" spans="2:7" ht="21" customHeight="1">
+    <row r="17" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="42" t="s">
+      <c r="C17" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="44"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="48"/>
     </row>
-    <row r="18" spans="2:7" ht="84" customHeight="1">
+    <row r="18" spans="2:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="42" t="s">
+      <c r="C18" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="43"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="44"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="48"/>
     </row>
-    <row r="19" spans="2:7" ht="33.75" customHeight="1">
+    <row r="19" spans="2:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="42" t="s">
+      <c r="C19" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="43"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="44"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="48"/>
     </row>
-    <row r="20" spans="2:7" ht="66" customHeight="1">
+    <row r="20" spans="2:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="42" t="s">
+      <c r="C20" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="44"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="48"/>
     </row>
-    <row r="21" spans="2:7" ht="36.75" customHeight="1">
+    <row r="21" spans="2:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="52" t="s">
+      <c r="C21" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="52"/>
-      <c r="E21" s="52"/>
-      <c r="F21" s="52"/>
-      <c r="G21" s="52"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="49"/>
     </row>
-    <row r="23" spans="2:7" ht="36.6" customHeight="1">
-      <c r="B23" s="48" t="s">
+    <row r="23" spans="2:7" ht="36.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="42" t="s">
+        <v>371</v>
+      </c>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="49"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="50" t="s">
-        <v>24</v>
-      </c>
-      <c r="F23" s="50"/>
-      <c r="G23" s="51"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
     <mergeCell ref="C15:G15"/>
     <mergeCell ref="C16:G16"/>
     <mergeCell ref="B1:G7"/>
@@ -8789,6 +8780,13 @@
     <mergeCell ref="C11:G11"/>
     <mergeCell ref="C13:G13"/>
     <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E23" r:id="rId1" display="https://creativecommons.org/licenses/by-nc-sa/3.0/igo" xr:uid="{09C8BD04-0482-4B35-B34C-0BD3D86441F2}"/>
@@ -8809,19 +8807,19 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="40.7109375" defaultRowHeight="12.95"/>
+  <sheetFormatPr defaultColWidth="40.7265625" defaultRowHeight="13" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.140625" style="22" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" style="22" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" style="22" customWidth="1"/>
-    <col min="4" max="4" width="34.5703125" style="22" customWidth="1"/>
-    <col min="5" max="9" width="40.7109375" style="22"/>
+    <col min="1" max="1" width="4.1796875" style="22" customWidth="1"/>
+    <col min="2" max="2" width="18.26953125" style="22" customWidth="1"/>
+    <col min="3" max="3" width="23.54296875" style="22" customWidth="1"/>
+    <col min="4" max="4" width="34.54296875" style="22" customWidth="1"/>
+    <col min="5" max="9" width="40.7265625" style="22"/>
     <col min="10" max="10" width="33" style="22" customWidth="1"/>
-    <col min="11" max="11" width="74.5703125" style="22" customWidth="1"/>
-    <col min="12" max="16384" width="40.7109375" style="22"/>
+    <col min="11" max="11" width="74.54296875" style="22" customWidth="1"/>
+    <col min="12" max="16384" width="40.7265625" style="22"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="14.45">
+    <row r="2" spans="2:12" ht="14.5" x14ac:dyDescent="0.25">
       <c r="B2" s="56" t="s">
         <v>3</v>
       </c>
@@ -8829,14 +8827,14 @@
         <v>5</v>
       </c>
       <c r="D2" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="56" t="s">
         <v>25</v>
-      </c>
-      <c r="E2" s="56" t="s">
-        <v>26</v>
       </c>
       <c r="F2" s="56"/>
       <c r="G2" s="59" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H2" s="59"/>
       <c r="I2" s="56" t="s">
@@ -8850,7 +8848,7 @@
       </c>
       <c r="L2" s="24"/>
     </row>
-    <row r="3" spans="2:12" ht="14.45">
+    <row r="3" spans="2:12" ht="14.5" x14ac:dyDescent="0.25">
       <c r="B3" s="56"/>
       <c r="C3" s="56"/>
       <c r="D3" s="58"/>
@@ -8858,1502 +8856,1502 @@
         <v>2</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G3" s="20" t="s">
         <v>2</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I3" s="56"/>
       <c r="J3" s="54"/>
       <c r="K3" s="55"/>
       <c r="L3" s="24"/>
     </row>
-    <row r="4" spans="2:12" ht="101.45">
+    <row r="4" spans="2:12" ht="87" x14ac:dyDescent="0.25">
       <c r="B4" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="D4" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="E4" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="F4" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="G4" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="H4" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="I4" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="I4" s="21" t="s">
+      <c r="J4" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="21" t="s">
+      <c r="K4" s="21" t="s">
         <v>37</v>
-      </c>
-      <c r="K4" s="21" t="s">
-        <v>38</v>
       </c>
       <c r="L4" s="24"/>
     </row>
-    <row r="5" spans="2:12" s="26" customFormat="1" ht="72.599999999999994">
+    <row r="5" spans="2:12" s="26" customFormat="1" ht="72.5" x14ac:dyDescent="0.25">
       <c r="B5" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="D5" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="E5" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="F5" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="21" t="s">
+      <c r="G5" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="J5" s="21" t="s">
+      <c r="K5" s="18" t="s">
         <v>44</v>
-      </c>
-      <c r="K5" s="18" t="s">
-        <v>45</v>
       </c>
       <c r="L5" s="25"/>
     </row>
-    <row r="6" spans="2:12" s="26" customFormat="1" ht="72.599999999999994">
+    <row r="6" spans="2:12" s="26" customFormat="1" ht="72.5" x14ac:dyDescent="0.25">
       <c r="B6" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="D6" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="E6" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="F6" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="G6" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="J6" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="G6" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="I6" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="J6" s="21" t="s">
+      <c r="K6" s="18" t="s">
         <v>51</v>
-      </c>
-      <c r="K6" s="18" t="s">
-        <v>52</v>
       </c>
       <c r="L6" s="25"/>
     </row>
-    <row r="7" spans="2:12" s="26" customFormat="1" ht="72.599999999999994">
+    <row r="7" spans="2:12" s="26" customFormat="1" ht="72.5" x14ac:dyDescent="0.25">
       <c r="B7" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="D7" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="E7" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="F7" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="F7" s="21" t="s">
+      <c r="G7" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="G7" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="I7" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="J7" s="21" t="s">
-        <v>58</v>
-      </c>
       <c r="K7" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L7" s="25"/>
     </row>
-    <row r="8" spans="2:12" ht="101.45">
+    <row r="8" spans="2:12" ht="87" x14ac:dyDescent="0.25">
       <c r="B8" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="D8" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="E8" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="F8" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="G8" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="G8" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="H8" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="I8" s="21" t="s">
+      <c r="J8" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="J8" s="21" t="s">
-        <v>65</v>
-      </c>
       <c r="K8" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L8" s="24"/>
     </row>
-    <row r="9" spans="2:12" s="26" customFormat="1" ht="72.599999999999994">
+    <row r="9" spans="2:12" s="26" customFormat="1" ht="72.5" x14ac:dyDescent="0.25">
       <c r="B9" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="D9" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="E9" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="F9" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="F9" s="21" t="s">
-        <v>70</v>
-      </c>
       <c r="G9" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="21" t="s">
+      <c r="I9" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="I9" s="21" t="s">
-        <v>36</v>
-      </c>
       <c r="J9" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K9" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L9" s="25"/>
     </row>
-    <row r="10" spans="2:12" s="26" customFormat="1" ht="72.599999999999994">
+    <row r="10" spans="2:12" s="26" customFormat="1" ht="72.5" x14ac:dyDescent="0.25">
       <c r="B10" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="D10" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="E10" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="F10" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="21" t="s">
-        <v>75</v>
-      </c>
       <c r="G10" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="H10" s="21" t="s">
+      <c r="I10" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="I10" s="21" t="s">
-        <v>36</v>
-      </c>
       <c r="J10" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K10" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L10" s="25"/>
     </row>
-    <row r="11" spans="2:12" s="26" customFormat="1" ht="72.599999999999994">
+    <row r="11" spans="2:12" s="26" customFormat="1" ht="72.5" x14ac:dyDescent="0.25">
       <c r="B11" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="D11" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="E11" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="F11" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="F11" s="21" t="s">
-        <v>80</v>
-      </c>
       <c r="G11" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="H11" s="21" t="s">
+      <c r="I11" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="I11" s="21" t="s">
-        <v>36</v>
-      </c>
       <c r="J11" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K11" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L11" s="25"/>
     </row>
-    <row r="12" spans="2:12" s="26" customFormat="1" ht="72.599999999999994">
+    <row r="12" spans="2:12" s="26" customFormat="1" ht="72.5" x14ac:dyDescent="0.25">
       <c r="B12" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="D12" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="E12" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="F12" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="F12" s="21" t="s">
-        <v>85</v>
-      </c>
       <c r="G12" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="H12" s="21" t="s">
+      <c r="I12" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="I12" s="21" t="s">
-        <v>36</v>
-      </c>
       <c r="J12" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K12" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L12" s="25"/>
     </row>
-    <row r="13" spans="2:12" s="26" customFormat="1" ht="72.599999999999994">
+    <row r="13" spans="2:12" s="26" customFormat="1" ht="72.5" x14ac:dyDescent="0.25">
       <c r="B13" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="D13" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="E13" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="F13" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="F13" s="21" t="s">
-        <v>90</v>
-      </c>
       <c r="G13" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="H13" s="21" t="s">
+      <c r="I13" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="I13" s="21" t="s">
-        <v>36</v>
-      </c>
       <c r="J13" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K13" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L13" s="25"/>
     </row>
-    <row r="14" spans="2:12" s="26" customFormat="1" ht="72.599999999999994">
+    <row r="14" spans="2:12" s="26" customFormat="1" ht="72.5" x14ac:dyDescent="0.25">
       <c r="B14" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="D14" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="E14" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="F14" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="F14" s="21" t="s">
-        <v>95</v>
-      </c>
       <c r="G14" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="H14" s="21" t="s">
+      <c r="I14" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="I14" s="21" t="s">
-        <v>36</v>
-      </c>
       <c r="J14" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K14" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L14" s="25"/>
     </row>
-    <row r="15" spans="2:12" s="29" customFormat="1" ht="72.599999999999994">
+    <row r="15" spans="2:12" s="29" customFormat="1" ht="72.5" x14ac:dyDescent="0.25">
       <c r="B15" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="D15" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="D15" s="21" t="s">
+      <c r="E15" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="E15" s="27" t="s">
+      <c r="F15" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="F15" s="27" t="s">
-        <v>100</v>
-      </c>
       <c r="G15" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="H15" s="21" t="s">
+      <c r="I15" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="I15" s="21" t="s">
-        <v>36</v>
-      </c>
       <c r="J15" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K15" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L15" s="28"/>
     </row>
-    <row r="16" spans="2:12" s="29" customFormat="1" ht="72.599999999999994">
+    <row r="16" spans="2:12" s="29" customFormat="1" ht="72.5" x14ac:dyDescent="0.25">
       <c r="B16" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="D16" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="D16" s="21" t="s">
+      <c r="E16" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="E16" s="27" t="s">
+      <c r="F16" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="F16" s="30" t="s">
-        <v>105</v>
-      </c>
       <c r="G16" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H16" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="H16" s="21" t="s">
+      <c r="I16" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="I16" s="21" t="s">
-        <v>36</v>
-      </c>
       <c r="J16" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K16" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L16" s="28"/>
     </row>
-    <row r="17" spans="2:12" s="26" customFormat="1" ht="57.95">
+    <row r="17" spans="2:12" s="26" customFormat="1" ht="58" x14ac:dyDescent="0.25">
       <c r="B17" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="D17" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="E17" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="E17" s="21" t="s">
+      <c r="F17" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="F17" s="21" t="s">
-        <v>110</v>
-      </c>
       <c r="G17" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H17" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="H17" s="21" t="s">
+      <c r="I17" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="I17" s="21" t="s">
-        <v>36</v>
-      </c>
       <c r="J17" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K17" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L17" s="25"/>
     </row>
-    <row r="18" spans="2:12" s="26" customFormat="1" ht="57.95">
+    <row r="18" spans="2:12" s="26" customFormat="1" ht="58" x14ac:dyDescent="0.25">
       <c r="B18" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="C18" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="D18" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="D18" s="21" t="s">
+      <c r="E18" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="E18" s="21" t="s">
+      <c r="F18" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="F18" s="21" t="s">
-        <v>115</v>
-      </c>
       <c r="G18" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="H18" s="21" t="s">
+      <c r="I18" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="I18" s="21" t="s">
-        <v>36</v>
-      </c>
       <c r="J18" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K18" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L18" s="25"/>
     </row>
-    <row r="19" spans="2:12" ht="101.45">
+    <row r="19" spans="2:12" ht="87" x14ac:dyDescent="0.25">
       <c r="B19" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="C19" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="D19" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="D19" s="21" t="s">
+      <c r="E19" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="E19" s="21" t="s">
+      <c r="F19" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="F19" s="21" t="s">
+      <c r="G19" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H19" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="I19" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="J19" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="G19" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="H19" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="I19" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="J19" s="21" t="s">
+      <c r="K19" s="21" t="s">
         <v>121</v>
-      </c>
-      <c r="K19" s="21" t="s">
-        <v>122</v>
       </c>
       <c r="L19" s="24"/>
     </row>
-    <row r="20" spans="2:12" ht="101.45">
+    <row r="20" spans="2:12" ht="87" x14ac:dyDescent="0.25">
       <c r="B20" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="C20" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="D20" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="D20" s="21" t="s">
+      <c r="E20" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="E20" s="21" t="s">
+      <c r="F20" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="F20" s="21" t="s">
+      <c r="G20" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H20" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="I20" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="J20" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="G20" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="H20" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="I20" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="J20" s="21" t="s">
+      <c r="K20" s="21" t="s">
         <v>128</v>
-      </c>
-      <c r="K20" s="21" t="s">
-        <v>129</v>
       </c>
       <c r="L20" s="24"/>
     </row>
-    <row r="21" spans="2:12" ht="101.45">
+    <row r="21" spans="2:12" ht="87" x14ac:dyDescent="0.25">
       <c r="B21" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="C21" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="C21" s="21" t="s">
+      <c r="D21" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="D21" s="21" t="s">
+      <c r="E21" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="E21" s="21" t="s">
+      <c r="F21" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="F21" s="21" t="s">
-        <v>134</v>
-      </c>
       <c r="G21" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H21" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="H21" s="21" t="s">
+      <c r="I21" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="I21" s="21" t="s">
-        <v>36</v>
-      </c>
       <c r="J21" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K21" s="21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L21" s="24"/>
     </row>
-    <row r="22" spans="2:12" ht="101.45">
+    <row r="22" spans="2:12" ht="87" x14ac:dyDescent="0.25">
       <c r="B22" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="C22" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="D22" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="D22" s="21" t="s">
+      <c r="E22" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="E22" s="21" t="s">
+      <c r="F22" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="F22" s="21" t="s">
+      <c r="G22" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H22" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="I22" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="J22" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="G22" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="H22" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="I22" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="J22" s="21" t="s">
-        <v>140</v>
-      </c>
       <c r="K22" s="21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L22" s="24"/>
     </row>
-    <row r="23" spans="2:12" ht="101.45">
+    <row r="23" spans="2:12" ht="87" x14ac:dyDescent="0.25">
       <c r="B23" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="C23" s="21" t="s">
         <v>141</v>
       </c>
-      <c r="C23" s="21" t="s">
+      <c r="D23" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="D23" s="21" t="s">
+      <c r="E23" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="E23" s="21" t="s">
+      <c r="F23" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="F23" s="21" t="s">
+      <c r="G23" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H23" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="I23" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="J23" s="21" t="s">
         <v>145</v>
       </c>
-      <c r="G23" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="H23" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="I23" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="J23" s="21" t="s">
+      <c r="K23" s="21" t="s">
         <v>146</v>
-      </c>
-      <c r="K23" s="21" t="s">
-        <v>147</v>
       </c>
       <c r="L23" s="24"/>
     </row>
-    <row r="24" spans="2:12" ht="72.599999999999994">
+    <row r="24" spans="2:12" ht="72.5" x14ac:dyDescent="0.25">
       <c r="B24" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="C24" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="C24" s="21" t="s">
+      <c r="D24" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="D24" s="21" t="s">
+      <c r="E24" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="E24" s="21" t="s">
+      <c r="F24" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="F24" s="21" t="s">
+      <c r="G24" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H24" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="I24" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="J24" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="G24" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="H24" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="I24" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="J24" s="21" t="s">
-        <v>153</v>
-      </c>
       <c r="K24" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L24" s="24"/>
     </row>
-    <row r="25" spans="2:12" s="26" customFormat="1" ht="72.599999999999994">
+    <row r="25" spans="2:12" s="26" customFormat="1" ht="72.5" x14ac:dyDescent="0.25">
       <c r="B25" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="C25" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="C25" s="21" t="s">
+      <c r="D25" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="D25" s="21" t="s">
+      <c r="E25" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="E25" s="21" t="s">
+      <c r="F25" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="F25" s="21" t="s">
-        <v>158</v>
-      </c>
       <c r="G25" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H25" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="H25" s="21" t="s">
+      <c r="I25" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="I25" s="21" t="s">
-        <v>36</v>
-      </c>
       <c r="J25" s="21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K25" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L25" s="25"/>
     </row>
-    <row r="26" spans="2:12" ht="72.599999999999994">
+    <row r="26" spans="2:12" ht="72.5" x14ac:dyDescent="0.25">
       <c r="B26" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="C26" s="21" t="s">
         <v>159</v>
       </c>
-      <c r="C26" s="21" t="s">
+      <c r="D26" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="D26" s="21" t="s">
+      <c r="E26" s="21" t="s">
         <v>161</v>
       </c>
-      <c r="E26" s="21" t="s">
+      <c r="F26" s="21" t="s">
         <v>162</v>
       </c>
-      <c r="F26" s="21" t="s">
-        <v>163</v>
-      </c>
       <c r="G26" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H26" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="H26" s="21" t="s">
+      <c r="I26" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="I26" s="21" t="s">
-        <v>36</v>
-      </c>
       <c r="J26" s="21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K26" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L26" s="24"/>
     </row>
-    <row r="27" spans="2:12" ht="72.599999999999994">
+    <row r="27" spans="2:12" ht="72.5" x14ac:dyDescent="0.25">
       <c r="B27" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="C27" s="21" t="s">
         <v>164</v>
       </c>
-      <c r="C27" s="21" t="s">
+      <c r="D27" s="21" t="s">
         <v>165</v>
       </c>
-      <c r="D27" s="21" t="s">
+      <c r="E27" s="21" t="s">
         <v>166</v>
       </c>
-      <c r="E27" s="21" t="s">
+      <c r="F27" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="F27" s="21" t="s">
-        <v>168</v>
-      </c>
       <c r="G27" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H27" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="H27" s="21" t="s">
+      <c r="I27" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="I27" s="21" t="s">
-        <v>36</v>
-      </c>
       <c r="J27" s="21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K27" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L27" s="24"/>
     </row>
-    <row r="28" spans="2:12" ht="72.599999999999994">
+    <row r="28" spans="2:12" ht="72.5" x14ac:dyDescent="0.25">
       <c r="B28" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="C28" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="C28" s="21" t="s">
+      <c r="D28" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="D28" s="21" t="s">
+      <c r="E28" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="E28" s="21" t="s">
+      <c r="F28" s="21" t="s">
         <v>172</v>
       </c>
-      <c r="F28" s="21" t="s">
-        <v>173</v>
-      </c>
       <c r="G28" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H28" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="H28" s="21" t="s">
+      <c r="I28" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="I28" s="21" t="s">
-        <v>36</v>
-      </c>
       <c r="J28" s="21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K28" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L28" s="24"/>
     </row>
-    <row r="29" spans="2:12" ht="101.45">
+    <row r="29" spans="2:12" ht="87" x14ac:dyDescent="0.25">
       <c r="B29" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="C29" s="21" t="s">
         <v>174</v>
       </c>
-      <c r="C29" s="21" t="s">
+      <c r="D29" s="21" t="s">
         <v>175</v>
       </c>
-      <c r="D29" s="21" t="s">
+      <c r="E29" s="21" t="s">
         <v>176</v>
       </c>
-      <c r="E29" s="21" t="s">
+      <c r="F29" s="21" t="s">
         <v>177</v>
       </c>
-      <c r="F29" s="21" t="s">
+      <c r="G29" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H29" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="I29" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="J29" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="G29" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="H29" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="I29" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="J29" s="21" t="s">
+      <c r="K29" s="21" t="s">
         <v>179</v>
-      </c>
-      <c r="K29" s="21" t="s">
-        <v>180</v>
       </c>
       <c r="L29" s="24"/>
     </row>
-    <row r="30" spans="2:12" ht="101.45">
+    <row r="30" spans="2:12" ht="87" x14ac:dyDescent="0.25">
       <c r="B30" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="C30" s="21" t="s">
         <v>181</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="D30" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="D30" s="21" t="s">
+      <c r="E30" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="E30" s="21" t="s">
+      <c r="F30" s="21" t="s">
         <v>184</v>
       </c>
-      <c r="F30" s="21" t="s">
+      <c r="G30" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H30" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="I30" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="J30" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="K30" s="21" t="s">
         <v>185</v>
-      </c>
-      <c r="G30" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="H30" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="I30" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="J30" s="21" t="s">
-        <v>179</v>
-      </c>
-      <c r="K30" s="21" t="s">
-        <v>186</v>
       </c>
       <c r="L30" s="24"/>
     </row>
-    <row r="31" spans="2:12" ht="101.45">
+    <row r="31" spans="2:12" ht="87" x14ac:dyDescent="0.25">
       <c r="B31" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="C31" s="21" t="s">
         <v>187</v>
       </c>
-      <c r="C31" s="21" t="s">
+      <c r="D31" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="D31" s="21" t="s">
+      <c r="E31" s="21" t="s">
         <v>189</v>
       </c>
-      <c r="E31" s="21" t="s">
+      <c r="F31" s="21" t="s">
         <v>190</v>
       </c>
-      <c r="F31" s="21" t="s">
-        <v>191</v>
-      </c>
       <c r="G31" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H31" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="H31" s="21" t="s">
+      <c r="I31" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="I31" s="21" t="s">
-        <v>36</v>
-      </c>
       <c r="J31" s="21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K31" s="21" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="L31" s="24"/>
     </row>
-    <row r="32" spans="2:12" s="29" customFormat="1" ht="101.45">
+    <row r="32" spans="2:12" s="29" customFormat="1" ht="87" x14ac:dyDescent="0.25">
       <c r="B32" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="C32" s="21" t="s">
         <v>192</v>
       </c>
-      <c r="C32" s="21" t="s">
+      <c r="D32" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="D32" s="21" t="s">
+      <c r="E32" s="21" t="s">
         <v>194</v>
       </c>
-      <c r="E32" s="21" t="s">
+      <c r="F32" s="21" t="s">
         <v>195</v>
       </c>
-      <c r="F32" s="21" t="s">
+      <c r="G32" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H32" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="I32" s="21" t="s">
         <v>196</v>
       </c>
-      <c r="G32" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="H32" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="I32" s="21" t="s">
-        <v>197</v>
-      </c>
       <c r="J32" s="21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K32" s="21" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="L32" s="28"/>
     </row>
-    <row r="33" spans="2:12" ht="101.45">
+    <row r="33" spans="2:12" ht="87" x14ac:dyDescent="0.25">
       <c r="B33" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="C33" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="C33" s="21" t="s">
+      <c r="D33" s="21" t="s">
         <v>199</v>
       </c>
-      <c r="D33" s="21" t="s">
+      <c r="E33" s="21" t="s">
         <v>200</v>
       </c>
-      <c r="E33" s="21" t="s">
+      <c r="F33" s="21" t="s">
         <v>201</v>
       </c>
-      <c r="F33" s="21" t="s">
+      <c r="G33" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H33" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="I33" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="J33" s="21" t="s">
         <v>202</v>
       </c>
-      <c r="G33" s="21" t="s">
+      <c r="K33" s="18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" ht="58" x14ac:dyDescent="0.25">
+      <c r="B34" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="C34" s="31" t="s">
+        <v>204</v>
+      </c>
+      <c r="D34" s="21" t="s">
+        <v>205</v>
+      </c>
+      <c r="E34" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="F34" s="21" t="s">
+        <v>207</v>
+      </c>
+      <c r="G34" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H34" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="H33" s="21" t="s">
+      <c r="I34" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="I33" s="21" t="s">
-        <v>197</v>
-      </c>
-      <c r="J33" s="21" t="s">
-        <v>203</v>
-      </c>
-      <c r="K33" s="18" t="s">
-        <v>52</v>
+      <c r="J34" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="K34" s="18" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="34" spans="2:12" ht="57.95">
-      <c r="B34" s="21" t="s">
-        <v>204</v>
-      </c>
-      <c r="C34" s="31" t="s">
-        <v>205</v>
-      </c>
-      <c r="D34" s="21" t="s">
-        <v>206</v>
-      </c>
-      <c r="E34" s="21" t="s">
-        <v>207</v>
-      </c>
-      <c r="F34" s="21" t="s">
+    <row r="35" spans="2:12" ht="58" x14ac:dyDescent="0.25">
+      <c r="B35" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="G34" s="21" t="s">
+      <c r="C35" s="21" t="s">
+        <v>209</v>
+      </c>
+      <c r="D35" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="E35" s="21" t="s">
+        <v>211</v>
+      </c>
+      <c r="F35" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="G35" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H35" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="H34" s="21" t="s">
+      <c r="I35" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="I34" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="J34" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="K34" s="18" t="s">
-        <v>52</v>
+      <c r="J35" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="K35" s="18" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="35" spans="2:12" ht="72.599999999999994">
-      <c r="B35" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="C35" s="21" t="s">
-        <v>210</v>
-      </c>
-      <c r="D35" s="21" t="s">
-        <v>211</v>
-      </c>
-      <c r="E35" s="21" t="s">
-        <v>212</v>
-      </c>
-      <c r="F35" s="21" t="s">
+    <row r="36" spans="2:12" ht="58" x14ac:dyDescent="0.25">
+      <c r="B36" s="21" t="s">
         <v>213</v>
       </c>
-      <c r="G35" s="21" t="s">
+      <c r="C36" s="21" t="s">
+        <v>214</v>
+      </c>
+      <c r="D36" s="21" t="s">
+        <v>215</v>
+      </c>
+      <c r="E36" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="F36" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="G36" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H36" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="H35" s="21" t="s">
+      <c r="I36" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="I35" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="J35" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="K35" s="18" t="s">
-        <v>52</v>
+      <c r="J36" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="K36" s="18" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="36" spans="2:12" ht="57.95">
-      <c r="B36" s="21" t="s">
-        <v>214</v>
-      </c>
-      <c r="C36" s="21" t="s">
-        <v>215</v>
-      </c>
-      <c r="D36" s="21" t="s">
-        <v>216</v>
-      </c>
-      <c r="E36" s="21" t="s">
-        <v>217</v>
-      </c>
-      <c r="F36" s="21" t="s">
+    <row r="37" spans="2:12" ht="58" x14ac:dyDescent="0.25">
+      <c r="B37" s="21" t="s">
         <v>218</v>
       </c>
-      <c r="G36" s="21" t="s">
+      <c r="C37" s="21" t="s">
+        <v>219</v>
+      </c>
+      <c r="D37" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="E37" s="21" t="s">
+        <v>221</v>
+      </c>
+      <c r="F37" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="G37" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H37" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="H36" s="21" t="s">
+      <c r="I37" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="I36" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="J36" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="K36" s="18" t="s">
-        <v>52</v>
+      <c r="J37" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="K37" s="18" t="s">
+        <v>51</v>
       </c>
     </row>
-    <row r="37" spans="2:12" ht="57.95">
-      <c r="B37" s="21" t="s">
-        <v>219</v>
-      </c>
-      <c r="C37" s="21" t="s">
-        <v>220</v>
-      </c>
-      <c r="D37" s="21" t="s">
-        <v>221</v>
-      </c>
-      <c r="E37" s="21" t="s">
-        <v>222</v>
-      </c>
-      <c r="F37" s="21" t="s">
+    <row r="38" spans="2:12" ht="130.5" x14ac:dyDescent="0.25">
+      <c r="B38" s="21" t="s">
         <v>223</v>
       </c>
-      <c r="G37" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="H37" s="21" t="s">
+      <c r="C38" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="D38" s="21" t="s">
+        <v>225</v>
+      </c>
+      <c r="E38" s="21" t="s">
+        <v>226</v>
+      </c>
+      <c r="F38" s="21" t="s">
+        <v>227</v>
+      </c>
+      <c r="G38" s="21" t="s">
+        <v>228</v>
+      </c>
+      <c r="H38" s="21" t="s">
+        <v>229</v>
+      </c>
+      <c r="I38" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="I37" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="J37" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="K37" s="18" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="38" spans="2:12" ht="130.5">
-      <c r="B38" s="21" t="s">
-        <v>224</v>
-      </c>
-      <c r="C38" s="21" t="s">
-        <v>225</v>
-      </c>
-      <c r="D38" s="21" t="s">
-        <v>226</v>
-      </c>
-      <c r="E38" s="21" t="s">
-        <v>227</v>
-      </c>
-      <c r="F38" s="21" t="s">
-        <v>228</v>
-      </c>
-      <c r="G38" s="21" t="s">
-        <v>229</v>
-      </c>
-      <c r="H38" s="21" t="s">
+      <c r="J38" s="21" t="s">
         <v>230</v>
       </c>
-      <c r="I38" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="J38" s="21" t="s">
-        <v>231</v>
-      </c>
       <c r="K38" s="38" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L38" s="24"/>
     </row>
-    <row r="39" spans="2:12" ht="130.5">
+    <row r="39" spans="2:12" ht="130.5" x14ac:dyDescent="0.25">
       <c r="B39" s="21" t="s">
+        <v>231</v>
+      </c>
+      <c r="C39" s="21" t="s">
         <v>232</v>
       </c>
-      <c r="C39" s="21" t="s">
+      <c r="D39" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="D39" s="21" t="s">
+      <c r="E39" s="21" t="s">
         <v>234</v>
       </c>
-      <c r="E39" s="21" t="s">
+      <c r="F39" s="21" t="s">
         <v>235</v>
       </c>
-      <c r="F39" s="21" t="s">
+      <c r="G39" s="21" t="s">
         <v>236</v>
       </c>
-      <c r="G39" s="21" t="s">
+      <c r="H39" s="21" t="s">
         <v>237</v>
       </c>
-      <c r="H39" s="21" t="s">
-        <v>238</v>
-      </c>
       <c r="I39" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J39" s="21" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="K39" s="38" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L39" s="24"/>
     </row>
-    <row r="40" spans="2:12" ht="144.94999999999999">
+    <row r="40" spans="2:12" ht="145" x14ac:dyDescent="0.25">
       <c r="B40" s="21" t="s">
+        <v>238</v>
+      </c>
+      <c r="C40" s="21" t="s">
         <v>239</v>
       </c>
-      <c r="C40" s="21" t="s">
+      <c r="D40" s="21" t="s">
         <v>240</v>
       </c>
-      <c r="D40" s="21" t="s">
+      <c r="E40" s="21" t="s">
         <v>241</v>
       </c>
-      <c r="E40" s="21" t="s">
+      <c r="F40" s="27" t="s">
         <v>242</v>
       </c>
-      <c r="F40" s="27" t="s">
+      <c r="G40" s="21" t="s">
         <v>243</v>
       </c>
-      <c r="G40" s="21" t="s">
+      <c r="H40" s="27" t="s">
         <v>244</v>
       </c>
-      <c r="H40" s="27" t="s">
-        <v>245</v>
-      </c>
       <c r="I40" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J40" s="21" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="K40" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L40" s="24"/>
     </row>
-    <row r="41" spans="2:12" s="26" customFormat="1" ht="130.5">
+    <row r="41" spans="2:12" s="26" customFormat="1" ht="130.5" x14ac:dyDescent="0.25">
       <c r="B41" s="21" t="s">
+        <v>245</v>
+      </c>
+      <c r="C41" s="31" t="s">
         <v>246</v>
       </c>
-      <c r="C41" s="31" t="s">
+      <c r="D41" s="21" t="s">
         <v>247</v>
       </c>
-      <c r="D41" s="21" t="s">
+      <c r="E41" s="21" t="s">
         <v>248</v>
       </c>
-      <c r="E41" s="21" t="s">
+      <c r="F41" s="21" t="s">
         <v>249</v>
       </c>
-      <c r="F41" s="21" t="s">
+      <c r="G41" s="21" t="s">
         <v>250</v>
       </c>
-      <c r="G41" s="21" t="s">
+      <c r="H41" s="21" t="s">
         <v>251</v>
       </c>
-      <c r="H41" s="21" t="s">
+      <c r="I41" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="J41" s="21" t="s">
         <v>252</v>
       </c>
-      <c r="I41" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="J41" s="21" t="s">
-        <v>253</v>
-      </c>
       <c r="K41" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L41" s="25"/>
     </row>
-    <row r="42" spans="2:12" s="26" customFormat="1" ht="130.5">
+    <row r="42" spans="2:12" s="26" customFormat="1" ht="130.5" x14ac:dyDescent="0.25">
       <c r="B42" s="21" t="s">
+        <v>253</v>
+      </c>
+      <c r="C42" s="21" t="s">
         <v>254</v>
       </c>
-      <c r="C42" s="21" t="s">
+      <c r="D42" s="21" t="s">
         <v>255</v>
       </c>
-      <c r="D42" s="21" t="s">
+      <c r="E42" s="21" t="s">
         <v>256</v>
       </c>
-      <c r="E42" s="21" t="s">
+      <c r="F42" s="21" t="s">
         <v>257</v>
       </c>
-      <c r="F42" s="21" t="s">
+      <c r="G42" s="21" t="s">
         <v>258</v>
       </c>
-      <c r="G42" s="21" t="s">
+      <c r="H42" s="21" t="s">
         <v>259</v>
       </c>
-      <c r="H42" s="21" t="s">
-        <v>260</v>
-      </c>
       <c r="I42" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J42" s="21" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="K42" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L42" s="25"/>
     </row>
-    <row r="43" spans="2:12" s="29" customFormat="1" ht="57.95">
+    <row r="43" spans="2:12" s="29" customFormat="1" ht="58" x14ac:dyDescent="0.25">
       <c r="B43" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="C43" s="21" t="s">
         <v>261</v>
       </c>
-      <c r="C43" s="21" t="s">
+      <c r="D43" s="21" t="s">
         <v>262</v>
       </c>
-      <c r="D43" s="21" t="s">
+      <c r="E43" s="21" t="s">
         <v>263</v>
       </c>
-      <c r="E43" s="21" t="s">
+      <c r="F43" s="21" t="s">
         <v>264</v>
       </c>
-      <c r="F43" s="21" t="s">
+      <c r="G43" s="21" t="s">
         <v>265</v>
       </c>
-      <c r="G43" s="21" t="s">
+      <c r="H43" s="21" t="s">
         <v>266</v>
       </c>
-      <c r="H43" s="21" t="s">
+      <c r="I43" s="21" t="s">
         <v>267</v>
       </c>
-      <c r="I43" s="21" t="s">
-        <v>268</v>
-      </c>
       <c r="J43" s="21" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="K43" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L43" s="28"/>
     </row>
-    <row r="44" spans="2:12" s="29" customFormat="1" ht="72.599999999999994">
+    <row r="44" spans="2:12" s="29" customFormat="1" ht="72.5" x14ac:dyDescent="0.25">
       <c r="B44" s="21" t="s">
+        <v>268</v>
+      </c>
+      <c r="C44" s="21" t="s">
         <v>269</v>
       </c>
-      <c r="C44" s="21" t="s">
+      <c r="D44" s="21" t="s">
         <v>270</v>
       </c>
-      <c r="D44" s="21" t="s">
+      <c r="E44" s="21" t="s">
         <v>271</v>
       </c>
-      <c r="E44" s="21" t="s">
+      <c r="F44" s="21" t="s">
         <v>272</v>
       </c>
-      <c r="F44" s="21" t="s">
+      <c r="G44" s="21" t="s">
         <v>273</v>
       </c>
-      <c r="G44" s="21" t="s">
+      <c r="H44" s="21" t="s">
         <v>274</v>
       </c>
-      <c r="H44" s="21" t="s">
+      <c r="I44" s="21" t="s">
         <v>275</v>
       </c>
-      <c r="I44" s="21" t="s">
+      <c r="J44" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="K44" s="21" t="s">
         <v>276</v>
-      </c>
-      <c r="J44" s="21" t="s">
-        <v>231</v>
-      </c>
-      <c r="K44" s="21" t="s">
-        <v>277</v>
       </c>
       <c r="L44" s="28"/>
     </row>
-    <row r="45" spans="2:12" s="29" customFormat="1" ht="144.94999999999999">
+    <row r="45" spans="2:12" s="29" customFormat="1" ht="145" x14ac:dyDescent="0.25">
       <c r="B45" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="C45" s="21" t="s">
         <v>278</v>
       </c>
-      <c r="C45" s="21" t="s">
+      <c r="D45" s="21" t="s">
         <v>279</v>
       </c>
-      <c r="D45" s="21" t="s">
+      <c r="E45" s="21" t="s">
         <v>280</v>
       </c>
-      <c r="E45" s="21" t="s">
+      <c r="F45" s="21" t="s">
         <v>281</v>
       </c>
-      <c r="F45" s="21" t="s">
+      <c r="G45" s="21" t="s">
         <v>282</v>
       </c>
-      <c r="G45" s="21" t="s">
+      <c r="H45" s="21" t="s">
         <v>283</v>
       </c>
-      <c r="H45" s="21" t="s">
+      <c r="I45" s="21" t="s">
         <v>284</v>
       </c>
-      <c r="I45" s="21" t="s">
+      <c r="J45" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="K45" s="21" t="s">
         <v>285</v>
-      </c>
-      <c r="J45" s="21" t="s">
-        <v>231</v>
-      </c>
-      <c r="K45" s="21" t="s">
-        <v>286</v>
       </c>
       <c r="L45" s="28"/>
     </row>
-    <row r="46" spans="2:12" s="29" customFormat="1" ht="87">
+    <row r="46" spans="2:12" s="29" customFormat="1" ht="87" x14ac:dyDescent="0.25">
       <c r="B46" s="21" t="s">
+        <v>286</v>
+      </c>
+      <c r="C46" s="21" t="s">
         <v>287</v>
       </c>
-      <c r="C46" s="21" t="s">
+      <c r="D46" s="21" t="s">
         <v>288</v>
       </c>
-      <c r="D46" s="21" t="s">
+      <c r="E46" s="21" t="s">
         <v>289</v>
       </c>
-      <c r="E46" s="21" t="s">
+      <c r="F46" s="21" t="s">
         <v>290</v>
       </c>
-      <c r="F46" s="21" t="s">
+      <c r="G46" s="21" t="s">
         <v>291</v>
       </c>
-      <c r="G46" s="21" t="s">
+      <c r="H46" s="21" t="s">
         <v>292</v>
       </c>
-      <c r="H46" s="21" t="s">
+      <c r="I46" s="21" t="s">
         <v>293</v>
       </c>
-      <c r="I46" s="21" t="s">
+      <c r="J46" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="K46" s="21" t="s">
         <v>294</v>
-      </c>
-      <c r="J46" s="21" t="s">
-        <v>231</v>
-      </c>
-      <c r="K46" s="21" t="s">
-        <v>295</v>
       </c>
       <c r="L46" s="28"/>
     </row>
-    <row r="47" spans="2:12" s="29" customFormat="1" ht="72.599999999999994">
+    <row r="47" spans="2:12" s="29" customFormat="1" ht="72.5" x14ac:dyDescent="0.25">
       <c r="B47" s="21" t="s">
+        <v>295</v>
+      </c>
+      <c r="C47" s="21" t="s">
         <v>296</v>
       </c>
-      <c r="C47" s="21" t="s">
+      <c r="D47" s="21" t="s">
         <v>297</v>
       </c>
-      <c r="D47" s="21" t="s">
+      <c r="E47" s="21" t="s">
         <v>298</v>
       </c>
-      <c r="E47" s="21" t="s">
+      <c r="F47" s="21" t="s">
         <v>299</v>
       </c>
-      <c r="F47" s="21" t="s">
+      <c r="G47" s="21" t="s">
         <v>300</v>
       </c>
-      <c r="G47" s="21" t="s">
+      <c r="H47" s="21" t="s">
+        <v>300</v>
+      </c>
+      <c r="I47" s="21" t="s">
         <v>301</v>
       </c>
-      <c r="H47" s="21" t="s">
-        <v>301</v>
-      </c>
-      <c r="I47" s="21" t="s">
-        <v>302</v>
-      </c>
       <c r="J47" s="21" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="K47" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L47" s="28"/>
     </row>
-    <row r="48" spans="2:12" s="29" customFormat="1" ht="43.5">
+    <row r="48" spans="2:12" s="29" customFormat="1" ht="43.5" x14ac:dyDescent="0.25">
       <c r="B48" s="21" t="s">
+        <v>302</v>
+      </c>
+      <c r="C48" s="21" t="s">
         <v>303</v>
       </c>
-      <c r="C48" s="21" t="s">
+      <c r="D48" s="21" t="s">
         <v>304</v>
       </c>
-      <c r="D48" s="21" t="s">
+      <c r="E48" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="E48" s="21" t="s">
+      <c r="F48" s="21" t="s">
         <v>306</v>
       </c>
-      <c r="F48" s="21" t="s">
+      <c r="G48" s="21" t="s">
         <v>307</v>
       </c>
-      <c r="G48" s="21" t="s">
+      <c r="H48" s="21" t="s">
         <v>308</v>
       </c>
-      <c r="H48" s="21" t="s">
+      <c r="I48" s="21" t="s">
         <v>309</v>
       </c>
-      <c r="I48" s="21" t="s">
-        <v>310</v>
-      </c>
       <c r="J48" s="21" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="K48" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L48" s="28"/>
     </row>
-    <row r="50" spans="2:11" ht="37.5" customHeight="1">
+    <row r="50" spans="2:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="53" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C50" s="53"/>
       <c r="D50" s="53"/>
@@ -10365,132 +10363,132 @@
       <c r="J50" s="53"/>
       <c r="K50" s="53"/>
     </row>
-    <row r="51" spans="2:11" ht="72.599999999999994">
+    <row r="51" spans="2:11" ht="72.5" x14ac:dyDescent="0.25">
       <c r="B51" s="32" t="s">
+        <v>311</v>
+      </c>
+      <c r="C51" s="32" t="s">
         <v>312</v>
       </c>
-      <c r="C51" s="32" t="s">
+      <c r="D51" s="21" t="s">
         <v>313</v>
       </c>
-      <c r="D51" s="21" t="s">
+      <c r="E51" s="21" t="s">
         <v>314</v>
       </c>
-      <c r="E51" s="21" t="s">
+      <c r="F51" s="21" t="s">
         <v>315</v>
       </c>
-      <c r="F51" s="21" t="s">
+      <c r="G51" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H51" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="I51" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="J51" s="32" t="s">
         <v>316</v>
       </c>
-      <c r="G51" s="21" t="s">
+      <c r="K51" s="23" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="52" spans="2:11" s="13" customFormat="1" ht="116" x14ac:dyDescent="0.25">
+      <c r="B52" s="32" t="s">
+        <v>311</v>
+      </c>
+      <c r="C52" s="32" t="s">
+        <v>318</v>
+      </c>
+      <c r="D52" s="32" t="s">
+        <v>319</v>
+      </c>
+      <c r="E52" s="21" t="s">
+        <v>320</v>
+      </c>
+      <c r="F52" s="32" t="s">
+        <v>321</v>
+      </c>
+      <c r="G52" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H52" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="H51" s="21" t="s">
+      <c r="I52" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="I51" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="J51" s="32" t="s">
+      <c r="J52" s="32" t="s">
+        <v>316</v>
+      </c>
+      <c r="K52" s="23" t="s">
         <v>317</v>
       </c>
-      <c r="K51" s="23" t="s">
-        <v>318</v>
-      </c>
     </row>
-    <row r="52" spans="2:11" s="13" customFormat="1" ht="116.1">
-      <c r="B52" s="32" t="s">
-        <v>312</v>
-      </c>
-      <c r="C52" s="32" t="s">
-        <v>319</v>
-      </c>
-      <c r="D52" s="32" t="s">
-        <v>320</v>
-      </c>
-      <c r="E52" s="21" t="s">
-        <v>321</v>
-      </c>
-      <c r="F52" s="32" t="s">
+    <row r="53" spans="2:11" s="13" customFormat="1" ht="87" x14ac:dyDescent="0.25">
+      <c r="B53" s="32" t="s">
+        <v>311</v>
+      </c>
+      <c r="C53" s="32" t="s">
         <v>322</v>
       </c>
-      <c r="G52" s="21" t="s">
+      <c r="D53" s="32" t="s">
+        <v>323</v>
+      </c>
+      <c r="E53" s="32" t="s">
+        <v>324</v>
+      </c>
+      <c r="F53" s="32" t="s">
+        <v>325</v>
+      </c>
+      <c r="G53" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H53" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="H52" s="21" t="s">
+      <c r="I53" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="I52" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="J52" s="32" t="s">
-        <v>317</v>
-      </c>
-      <c r="K52" s="23" t="s">
-        <v>318</v>
+      <c r="J53" s="32" t="s">
+        <v>316</v>
+      </c>
+      <c r="K53" s="32" t="s">
+        <v>326</v>
       </c>
     </row>
-    <row r="53" spans="2:11" s="13" customFormat="1" ht="87">
-      <c r="B53" s="32" t="s">
-        <v>312</v>
-      </c>
-      <c r="C53" s="32" t="s">
-        <v>323</v>
-      </c>
-      <c r="D53" s="32" t="s">
-        <v>324</v>
-      </c>
-      <c r="E53" s="32" t="s">
-        <v>325</v>
-      </c>
-      <c r="F53" s="32" t="s">
-        <v>326</v>
-      </c>
-      <c r="G53" s="21" t="s">
+    <row r="54" spans="2:11" s="13" customFormat="1" ht="145" x14ac:dyDescent="0.25">
+      <c r="B54" s="32" t="s">
+        <v>311</v>
+      </c>
+      <c r="C54" s="32" t="s">
+        <v>327</v>
+      </c>
+      <c r="D54" s="32" t="s">
+        <v>328</v>
+      </c>
+      <c r="E54" s="32" t="s">
+        <v>329</v>
+      </c>
+      <c r="F54" s="32" t="s">
+        <v>330</v>
+      </c>
+      <c r="G54" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="H54" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="H53" s="21" t="s">
+      <c r="I54" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="I53" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="J53" s="32" t="s">
-        <v>317</v>
-      </c>
-      <c r="K53" s="32" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="54" spans="2:11" s="13" customFormat="1" ht="144.94999999999999">
-      <c r="B54" s="32" t="s">
-        <v>312</v>
-      </c>
-      <c r="C54" s="32" t="s">
-        <v>328</v>
-      </c>
-      <c r="D54" s="32" t="s">
-        <v>329</v>
-      </c>
-      <c r="E54" s="32" t="s">
-        <v>330</v>
-      </c>
-      <c r="F54" s="32" t="s">
+      <c r="J54" s="32" t="s">
+        <v>316</v>
+      </c>
+      <c r="K54" s="32" t="s">
         <v>331</v>
-      </c>
-      <c r="G54" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="H54" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="I54" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="J54" s="32" t="s">
-        <v>317</v>
-      </c>
-      <c r="K54" s="32" t="s">
-        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -10520,330 +10518,325 @@
       <selection activeCell="J35" sqref="A1:J35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.6"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="1" max="1" width="3.1796875" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10">
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
     </row>
-    <row r="2" spans="2:10">
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="61"/>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
     </row>
-    <row r="3" spans="2:10">
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="61"/>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
     </row>
-    <row r="4" spans="2:10">
-      <c r="B4" s="61"/>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="61"/>
-      <c r="I4" s="61"/>
-      <c r="J4" s="61"/>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="63"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="63"/>
     </row>
-    <row r="5" spans="2:10">
-      <c r="B5" s="61"/>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="61"/>
-      <c r="H5" s="61"/>
-      <c r="I5" s="61"/>
-      <c r="J5" s="61"/>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="63"/>
     </row>
-    <row r="6" spans="2:10">
-      <c r="B6" s="61"/>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="61"/>
-      <c r="I6" s="61"/>
-      <c r="J6" s="61"/>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="63"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
     </row>
-    <row r="7" spans="2:10">
-      <c r="B7" s="61"/>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="61"/>
-      <c r="G7" s="61"/>
-      <c r="H7" s="61"/>
-      <c r="I7" s="61"/>
-      <c r="J7" s="61"/>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="63"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="63"/>
+      <c r="I7" s="63"/>
+      <c r="J7" s="63"/>
     </row>
-    <row r="8" spans="2:10">
-      <c r="B8" s="61"/>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="61"/>
-      <c r="G8" s="61"/>
-      <c r="H8" s="61"/>
-      <c r="I8" s="61"/>
-      <c r="J8" s="61"/>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="63"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="63"/>
+      <c r="H8" s="63"/>
+      <c r="I8" s="63"/>
+      <c r="J8" s="63"/>
     </row>
-    <row r="9" spans="2:10" ht="12.95">
+    <row r="9" spans="2:10" ht="13" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="C9" s="64" t="s">
         <v>333</v>
       </c>
-      <c r="C9" s="62" t="s">
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="64"/>
+      <c r="H9" s="64"/>
+      <c r="I9" s="64"/>
+      <c r="J9" s="64"/>
+    </row>
+    <row r="10" spans="2:10" ht="13" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="D9" s="62"/>
-      <c r="E9" s="62"/>
-      <c r="F9" s="62"/>
-      <c r="G9" s="62"/>
-      <c r="H9" s="62"/>
-      <c r="I9" s="62"/>
-      <c r="J9" s="62"/>
+      <c r="C10" s="64" t="s">
+        <v>335</v>
+      </c>
+      <c r="D10" s="64"/>
+      <c r="E10" s="64"/>
+      <c r="F10" s="64"/>
+      <c r="G10" s="64"/>
+      <c r="H10" s="64"/>
+      <c r="I10" s="64"/>
+      <c r="J10" s="64"/>
     </row>
-    <row r="10" spans="2:10" ht="12.95">
-      <c r="B10" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="C10" s="62" t="s">
+    <row r="11" spans="2:10" ht="13" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="D10" s="62"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="62"/>
-      <c r="G10" s="62"/>
-      <c r="H10" s="62"/>
-      <c r="I10" s="62"/>
-      <c r="J10" s="62"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="64"/>
+      <c r="H11" s="64"/>
+      <c r="I11" s="64"/>
+      <c r="J11" s="64"/>
     </row>
-    <row r="11" spans="2:10" ht="12.95">
-      <c r="B11" s="2" t="s">
+    <row r="12" spans="2:10" ht="13" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="2:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="C11" s="62"/>
-      <c r="D11" s="62"/>
-      <c r="E11" s="62"/>
-      <c r="F11" s="62"/>
-      <c r="G11" s="62"/>
-      <c r="H11" s="62"/>
-      <c r="I11" s="62"/>
-      <c r="J11" s="62"/>
+      <c r="C13" s="62" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="62"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="62"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="62"/>
     </row>
-    <row r="12" spans="2:10" ht="12.95" thickBot="1"/>
-    <row r="13" spans="2:10" ht="14.1" thickTop="1" thickBot="1">
-      <c r="B13" s="3" t="s">
+    <row r="14" spans="2:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="C13" s="60" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="60"/>
-      <c r="E13" s="60"/>
-      <c r="F13" s="60"/>
-      <c r="G13" s="60"/>
-      <c r="H13" s="60"/>
-      <c r="I13" s="60"/>
-      <c r="J13" s="60"/>
+      <c r="C14" s="65" t="s">
+        <v>339</v>
+      </c>
+      <c r="D14" s="60"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="60"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="60"/>
     </row>
-    <row r="14" spans="2:10" ht="14.1" thickTop="1" thickBot="1">
-      <c r="B14" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="C14" s="63" t="s">
+    <row r="15" spans="2:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="5" t="s">
         <v>340</v>
       </c>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="64"/>
-      <c r="G14" s="64"/>
-      <c r="H14" s="64"/>
-      <c r="I14" s="64"/>
-      <c r="J14" s="64"/>
+      <c r="C15" s="60" t="s">
+        <v>341</v>
+      </c>
+      <c r="D15" s="60"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="60"/>
+      <c r="H15" s="60"/>
+      <c r="I15" s="60"/>
+      <c r="J15" s="60"/>
     </row>
-    <row r="15" spans="2:10" ht="14.1" thickTop="1" thickBot="1">
-      <c r="B15" s="5" t="s">
-        <v>341</v>
-      </c>
-      <c r="C15" s="64" t="s">
-        <v>342</v>
-      </c>
-      <c r="D15" s="64"/>
-      <c r="E15" s="64"/>
-      <c r="F15" s="64"/>
-      <c r="G15" s="64"/>
-      <c r="H15" s="64"/>
-      <c r="I15" s="64"/>
-      <c r="J15" s="64"/>
+    <row r="16" spans="2:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="5"/>
+      <c r="C16" s="61"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="61"/>
+      <c r="H16" s="61"/>
+      <c r="I16" s="61"/>
+      <c r="J16" s="61"/>
     </row>
-    <row r="16" spans="2:10" ht="14.1" thickTop="1" thickBot="1">
-      <c r="B16" s="5"/>
-      <c r="C16" s="65"/>
-      <c r="D16" s="65"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="65"/>
-      <c r="G16" s="65"/>
-      <c r="H16" s="65"/>
-      <c r="I16" s="65"/>
-      <c r="J16" s="65"/>
-    </row>
-    <row r="17" spans="1:13" ht="14.1" thickTop="1" thickBot="1">
+    <row r="17" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="6"/>
-      <c r="C17" s="65"/>
-      <c r="D17" s="65"/>
-      <c r="E17" s="65"/>
-      <c r="F17" s="65"/>
-      <c r="G17" s="65"/>
-      <c r="H17" s="65"/>
-      <c r="I17" s="65"/>
-      <c r="J17" s="65"/>
+      <c r="C17" s="61"/>
+      <c r="D17" s="61"/>
+      <c r="E17" s="61"/>
+      <c r="F17" s="61"/>
+      <c r="G17" s="61"/>
+      <c r="H17" s="61"/>
+      <c r="I17" s="61"/>
+      <c r="J17" s="61"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="1:13" ht="14.1" thickTop="1" thickBot="1">
+    <row r="18" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="5"/>
-      <c r="C18" s="64"/>
-      <c r="D18" s="64"/>
-      <c r="E18" s="64"/>
-      <c r="F18" s="64"/>
-      <c r="G18" s="64"/>
-      <c r="H18" s="64"/>
-      <c r="I18" s="64"/>
-      <c r="J18" s="64"/>
+      <c r="C18" s="60"/>
+      <c r="D18" s="60"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="60"/>
     </row>
-    <row r="19" spans="1:13" ht="30.75" customHeight="1" thickTop="1" thickBot="1">
+    <row r="19" spans="1:13" ht="30.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="C19" s="66" t="s">
         <v>343</v>
       </c>
-      <c r="C19" s="66" t="s">
+      <c r="D19" s="61"/>
+      <c r="E19" s="61"/>
+      <c r="F19" s="61"/>
+      <c r="G19" s="61"/>
+      <c r="H19" s="61"/>
+      <c r="I19" s="61"/>
+      <c r="J19" s="61"/>
+    </row>
+    <row r="20" spans="1:13" ht="13.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="D19" s="65"/>
-      <c r="E19" s="65"/>
-      <c r="F19" s="65"/>
-      <c r="G19" s="65"/>
-      <c r="H19" s="65"/>
-      <c r="I19" s="65"/>
-      <c r="J19" s="65"/>
+      <c r="C21" s="62" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="62"/>
+      <c r="E21" s="62"/>
+      <c r="F21" s="62"/>
+      <c r="G21" s="62"/>
+      <c r="H21" s="62"/>
+      <c r="I21" s="62"/>
+      <c r="J21" s="62"/>
     </row>
-    <row r="20" spans="1:13" ht="13.5" thickTop="1" thickBot="1"/>
-    <row r="21" spans="1:13" ht="14.1" thickTop="1" thickBot="1">
-      <c r="B21" s="3" t="s">
+    <row r="22" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="8"/>
+      <c r="C22" s="60"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="60"/>
+      <c r="F22" s="60"/>
+      <c r="G22" s="60"/>
+      <c r="H22" s="60"/>
+      <c r="I22" s="60"/>
+      <c r="J22" s="60"/>
+    </row>
+    <row r="23" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="9"/>
+      <c r="C23" s="60"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="60"/>
+      <c r="F23" s="60"/>
+      <c r="G23" s="60"/>
+      <c r="H23" s="60"/>
+      <c r="I23" s="60"/>
+      <c r="J23" s="60"/>
+    </row>
+    <row r="24" spans="1:13" ht="40.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="10"/>
+      <c r="C24" s="61" t="s">
         <v>345</v>
       </c>
-      <c r="C21" s="60" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" s="60"/>
-      <c r="E21" s="60"/>
-      <c r="F21" s="60"/>
-      <c r="G21" s="60"/>
-      <c r="H21" s="60"/>
-      <c r="I21" s="60"/>
-      <c r="J21" s="60"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="61"/>
+      <c r="F24" s="61"/>
+      <c r="G24" s="61"/>
+      <c r="H24" s="61"/>
+      <c r="I24" s="61"/>
+      <c r="J24" s="61"/>
     </row>
-    <row r="22" spans="1:13" ht="14.1" thickTop="1" thickBot="1">
-      <c r="B22" s="8"/>
-      <c r="C22" s="64"/>
-      <c r="D22" s="64"/>
-      <c r="E22" s="64"/>
-      <c r="F22" s="64"/>
-      <c r="G22" s="64"/>
-      <c r="H22" s="64"/>
-      <c r="I22" s="64"/>
-      <c r="J22" s="64"/>
+    <row r="25" spans="1:13" ht="27.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="11" t="s">
+        <v>346</v>
+      </c>
+      <c r="C25" s="61" t="s">
+        <v>347</v>
+      </c>
+      <c r="D25" s="61"/>
+      <c r="E25" s="61"/>
+      <c r="F25" s="61"/>
+      <c r="G25" s="61"/>
+      <c r="H25" s="61"/>
+      <c r="I25" s="61"/>
+      <c r="J25" s="61"/>
     </row>
-    <row r="23" spans="1:13" ht="14.1" thickTop="1" thickBot="1">
-      <c r="B23" s="9"/>
-      <c r="C23" s="64"/>
-      <c r="D23" s="64"/>
-      <c r="E23" s="64"/>
-      <c r="F23" s="64"/>
-      <c r="G23" s="64"/>
-      <c r="H23" s="64"/>
-      <c r="I23" s="64"/>
-      <c r="J23" s="64"/>
+    <row r="26" spans="1:13" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="12" t="s">
+        <v>346</v>
+      </c>
+      <c r="C26" s="60" t="s">
+        <v>348</v>
+      </c>
+      <c r="D26" s="60"/>
+      <c r="E26" s="60"/>
+      <c r="F26" s="60"/>
+      <c r="G26" s="60"/>
+      <c r="H26" s="60"/>
+      <c r="I26" s="60"/>
+      <c r="J26" s="60"/>
     </row>
-    <row r="24" spans="1:13" ht="40.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B24" s="10"/>
-      <c r="C24" s="65" t="s">
-        <v>346</v>
-      </c>
-      <c r="D24" s="65"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="65"/>
-      <c r="G24" s="65"/>
-      <c r="H24" s="65"/>
-      <c r="I24" s="65"/>
-      <c r="J24" s="65"/>
-    </row>
-    <row r="25" spans="1:13" ht="27.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B25" s="11" t="s">
-        <v>347</v>
-      </c>
-      <c r="C25" s="65" t="s">
-        <v>348</v>
-      </c>
-      <c r="D25" s="65"/>
-      <c r="E25" s="65"/>
-      <c r="F25" s="65"/>
-      <c r="G25" s="65"/>
-      <c r="H25" s="65"/>
-      <c r="I25" s="65"/>
-      <c r="J25" s="65"/>
-    </row>
-    <row r="26" spans="1:13" ht="14.1" thickTop="1" thickBot="1">
-      <c r="B26" s="12" t="s">
-        <v>347</v>
-      </c>
-      <c r="C26" s="64" t="s">
-        <v>349</v>
-      </c>
-      <c r="D26" s="64"/>
-      <c r="E26" s="64"/>
-      <c r="F26" s="64"/>
-      <c r="G26" s="64"/>
-      <c r="H26" s="64"/>
-      <c r="I26" s="64"/>
-      <c r="J26" s="64"/>
-    </row>
-    <row r="27" spans="1:13" ht="12.95" thickTop="1"/>
+    <row r="27" spans="1:13" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C22:J22"/>
-    <mergeCell ref="C23:J23"/>
-    <mergeCell ref="C24:J24"/>
-    <mergeCell ref="C25:J25"/>
-    <mergeCell ref="C26:J26"/>
     <mergeCell ref="C21:J21"/>
     <mergeCell ref="B1:J8"/>
     <mergeCell ref="C9:J9"/>
@@ -10856,6 +10849,11 @@
     <mergeCell ref="C17:J17"/>
     <mergeCell ref="C18:J18"/>
     <mergeCell ref="C19:J19"/>
+    <mergeCell ref="C22:J22"/>
+    <mergeCell ref="C23:J23"/>
+    <mergeCell ref="C24:J24"/>
+    <mergeCell ref="C25:J25"/>
+    <mergeCell ref="C26:J26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10871,115 +10869,115 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="35" customWidth="1"/>
-    <col min="2" max="2" width="4.140625" style="35" customWidth="1"/>
-    <col min="3" max="3" width="78.7109375" style="35" customWidth="1"/>
-    <col min="4" max="4" width="61.7109375" style="35" customWidth="1"/>
-    <col min="5" max="5" width="98.28515625" style="36" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="35"/>
+    <col min="1" max="1" width="3.26953125" style="35" customWidth="1"/>
+    <col min="2" max="2" width="4.1796875" style="35" customWidth="1"/>
+    <col min="3" max="3" width="78.7265625" style="35" customWidth="1"/>
+    <col min="4" max="4" width="61.7265625" style="35" customWidth="1"/>
+    <col min="5" max="5" width="98.26953125" style="36" customWidth="1"/>
+    <col min="6" max="16384" width="9.1796875" style="35"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="20.25" customHeight="1">
+    <row r="2" spans="2:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="33"/>
       <c r="C2" s="34" t="s">
+        <v>349</v>
+      </c>
+      <c r="D2" s="34" t="s">
         <v>350</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="E2" s="34" t="s">
         <v>351</v>
       </c>
-      <c r="E2" s="34" t="s">
-        <v>352</v>
-      </c>
     </row>
-    <row r="3" spans="2:5" ht="76.900000000000006" customHeight="1">
+    <row r="3" spans="2:5" ht="76.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="36">
         <v>1</v>
       </c>
       <c r="C3" s="36" t="s">
+        <v>352</v>
+      </c>
+      <c r="D3" s="36" t="s">
         <v>353</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="E3" s="37" t="s">
         <v>354</v>
       </c>
-      <c r="E3" s="37" t="s">
-        <v>355</v>
-      </c>
     </row>
-    <row r="4" spans="2:5" ht="42" customHeight="1">
+    <row r="4" spans="2:5" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="36">
         <v>2</v>
       </c>
       <c r="C4" s="36" t="s">
+        <v>355</v>
+      </c>
+      <c r="D4" s="35" t="s">
         <v>356</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="E4" s="37" t="s">
         <v>357</v>
       </c>
-      <c r="E4" s="37" t="s">
-        <v>358</v>
-      </c>
     </row>
-    <row r="5" spans="2:5" ht="36" customHeight="1">
+    <row r="5" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="36">
         <v>3</v>
       </c>
       <c r="C5" s="36" t="s">
+        <v>358</v>
+      </c>
+      <c r="D5" s="35" t="s">
         <v>359</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="E5" s="36" t="s">
         <v>360</v>
       </c>
-      <c r="E5" s="36" t="s">
-        <v>361</v>
-      </c>
     </row>
-    <row r="6" spans="2:5" ht="66.599999999999994" customHeight="1">
+    <row r="6" spans="2:5" ht="66.650000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="36">
         <v>4</v>
       </c>
       <c r="C6" s="36" t="s">
+        <v>361</v>
+      </c>
+      <c r="D6" s="35" t="s">
         <v>362</v>
       </c>
-      <c r="D6" s="35" t="s">
+      <c r="E6" s="37" t="s">
         <v>363</v>
       </c>
-      <c r="E6" s="37" t="s">
-        <v>364</v>
-      </c>
     </row>
-    <row r="7" spans="2:5" ht="66.599999999999994" customHeight="1">
+    <row r="7" spans="2:5" ht="66.650000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="36">
         <v>5</v>
       </c>
       <c r="C7" s="36" t="s">
+        <v>364</v>
+      </c>
+      <c r="D7" s="35" t="s">
         <v>365</v>
       </c>
-      <c r="D7" s="35" t="s">
+      <c r="E7" s="40" t="s">
         <v>366</v>
       </c>
-      <c r="E7" s="40" t="s">
-        <v>367</v>
-      </c>
     </row>
-    <row r="8" spans="2:5" ht="43.5">
+    <row r="8" spans="2:5" ht="43.5" x14ac:dyDescent="0.25">
       <c r="B8" s="35">
         <v>6</v>
       </c>
       <c r="C8" s="36" t="s">
+        <v>367</v>
+      </c>
+      <c r="D8" s="35" t="s">
         <v>368</v>
       </c>
-      <c r="D8" s="35" t="s">
+      <c r="E8" s="37" t="s">
         <v>369</v>
       </c>
-      <c r="E8" s="37" t="s">
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="39" t="s">
         <v>370</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5">
-      <c r="C10" s="39" t="s">
-        <v>371</v>
       </c>
     </row>
   </sheetData>
@@ -11006,114 +11004,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="51983ca6-de84-41fa-9a65-1d08ee1009bc">
-      <UserInfo>
-        <DisplayName>NASH-MENDEZ, Natschja</DisplayName>
-        <AccountId>7</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Pete Christopher (Green Ink) (p.christopher@greenink.co.uk)</DisplayName>
-        <AccountId>26</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BARREIX ETCHEGOIMBERRY, Maria</DisplayName>
-        <AccountId>13</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>AMIN, Avni</DisplayName>
-        <AccountId>46</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>GARCIA MORENO ESTEVA, Claudia M.</DisplayName>
-        <AccountId>47</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>KIPRUTO, Hillary Kipchumba</DisplayName>
-        <AccountId>28</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>SEYDI, Aminata Binetou Wahebine</DisplayName>
-        <AccountId>61</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>TITI-OFEI, Regina</DisplayName>
-        <AccountId>62</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>COSMAS, Leonard</DisplayName>
-        <AccountId>63</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>GACIC-DOBO, Marta</DisplayName>
-        <AccountId>450</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>PALLIWAL, Akshita</DisplayName>
-        <AccountId>155</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>DANOVARO, M. Carolina</DisplayName>
-        <AccountId>440</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Laura NIC LOCHLAINN</DisplayName>
-        <AccountId>457</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>GREVENDONK, Jan</DisplayName>
-        <AccountId>23</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>GOODMAN, Tracey S.</DisplayName>
-        <AccountId>236</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>SHENDALE, Stephanie</DisplayName>
-        <AccountId>452</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>CORMAN, Constantin</DisplayName>
-        <AccountId>200</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BROOKS, Donald Joseph</DisplayName>
-        <AccountId>421</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>MEHL, Garrett Livingston</DisplayName>
-        <AccountId>22</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <TaxCatchAll xmlns="51983ca6-de84-41fa-9a65-1d08ee1009bc" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="73389989-ac93-4f39-a9f3-2949bbf25fcc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008A6DDC313EDC9A43B330D8B6305883A5" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a5b0342cd22268e5e5d3683a3cff816e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="73389989-ac93-4f39-a9f3-2949bbf25fcc" xmlns:ns3="51983ca6-de84-41fa-9a65-1d08ee1009bc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c638d06e48d95e9efa3bb75773f50cd7" ns2:_="" ns3:_="">
     <xsd:import namespace="73389989-ac93-4f39-a9f3-2949bbf25fcc"/>
@@ -11368,14 +11258,148 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="51983ca6-de84-41fa-9a65-1d08ee1009bc">
+      <UserInfo>
+        <DisplayName>NASH-MENDEZ, Natschja</DisplayName>
+        <AccountId>7</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Pete Christopher (Green Ink) (p.christopher@greenink.co.uk)</DisplayName>
+        <AccountId>26</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BARREIX ETCHEGOIMBERRY, Maria</DisplayName>
+        <AccountId>13</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>AMIN, Avni</DisplayName>
+        <AccountId>46</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>GARCIA MORENO ESTEVA, Claudia M.</DisplayName>
+        <AccountId>47</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>KIPRUTO, Hillary Kipchumba</DisplayName>
+        <AccountId>28</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>SEYDI, Aminata Binetou Wahebine</DisplayName>
+        <AccountId>61</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>TITI-OFEI, Regina</DisplayName>
+        <AccountId>62</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>COSMAS, Leonard</DisplayName>
+        <AccountId>63</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>GACIC-DOBO, Marta</DisplayName>
+        <AccountId>450</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>PALLIWAL, Akshita</DisplayName>
+        <AccountId>155</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>DANOVARO, M. Carolina</DisplayName>
+        <AccountId>440</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Laura NIC LOCHLAINN</DisplayName>
+        <AccountId>457</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>GREVENDONK, Jan</DisplayName>
+        <AccountId>23</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>GOODMAN, Tracey S.</DisplayName>
+        <AccountId>236</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>SHENDALE, Stephanie</DisplayName>
+        <AccountId>452</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>CORMAN, Constantin</DisplayName>
+        <AccountId>200</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BROOKS, Donald Joseph</DisplayName>
+        <AccountId>421</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>MEHL, Garrett Livingston</DisplayName>
+        <AccountId>22</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <TaxCatchAll xmlns="51983ca6-de84-41fa-9a65-1d08ee1009bc" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="73389989-ac93-4f39-a9f3-2949bbf25fcc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3641399-1C83-4230-9FA0-63883702B763}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3641399-1C83-4230-9FA0-63883702B763}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5128250D-9B2C-4D86-9D99-709881CA8B0F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A29C1B64-DB83-4B97-8EAD-907E8399AE04}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="73389989-ac93-4f39-a9f3-2949bbf25fcc"/>
+    <ds:schemaRef ds:uri="51983ca6-de84-41fa-9a65-1d08ee1009bc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A29C1B64-DB83-4B97-8EAD-907E8399AE04}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5128250D-9B2C-4D86-9D99-709881CA8B0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="51983ca6-de84-41fa-9a65-1d08ee1009bc"/>
+    <ds:schemaRef ds:uri="73389989-ac93-4f39-a9f3-2949bbf25fcc"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>